<commit_message>
1 Add CityItemData structure 2 Small change in ItemBrowsePanel
</commit_message>
<xml_diff>
--- a/DataSource/excel/city.xlsx
+++ b/DataSource/excel/city.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="0" windowWidth="21200" windowHeight="14900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1200" yWindow="1200" windowWidth="24400" windowHeight="13680" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -199,12 +199,46 @@
         </r>
       </text>
     </comment>
+    <comment ref="U1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yujie Liu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t>贩卖的道具ID，卖掉之后就不再有这个商品了，如果玩家把道具卖入城市，则城市又会出现该道具</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="227">
   <si>
     <t>cityId</t>
   </si>
@@ -879,6 +913,12 @@
   </si>
   <si>
     <t>6;16;53;13</t>
+  </si>
+  <si>
+    <t>sellItemId</t>
+  </si>
+  <si>
+    <t>1;2</t>
   </si>
 </sst>
 </file>
@@ -1358,13 +1398,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T95"/>
+  <dimension ref="A1:U95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J38" sqref="J38"/>
+      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1378,7 +1418,7 @@
     <col min="20" max="20" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1439,8 +1479,11 @@
       <c r="T1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1501,8 +1544,11 @@
       <c r="T2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1563,8 +1609,11 @@
       <c r="T3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1625,8 +1674,11 @@
       <c r="T4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1687,8 +1739,11 @@
       <c r="T5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1749,8 +1804,11 @@
       <c r="T6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1811,8 +1869,11 @@
       <c r="T7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1873,8 +1934,11 @@
       <c r="T8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1935,8 +1999,11 @@
       <c r="T9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="U9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1997,8 +2064,11 @@
       <c r="T10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2059,8 +2129,11 @@
       <c r="T11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="U11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2121,8 +2194,11 @@
       <c r="T12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2183,8 +2259,11 @@
       <c r="T13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="U13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2245,8 +2324,11 @@
       <c r="T14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="U14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2307,8 +2389,11 @@
       <c r="T15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="U15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2369,8 +2454,11 @@
       <c r="T16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="U16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2431,8 +2519,11 @@
       <c r="T17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="U17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2493,8 +2584,11 @@
       <c r="T18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="U18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2555,8 +2649,11 @@
       <c r="T19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="U19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2617,8 +2714,11 @@
       <c r="T20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="U20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2679,8 +2779,11 @@
       <c r="T21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="U21" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2741,8 +2844,11 @@
       <c r="T22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="U22" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2803,8 +2909,11 @@
       <c r="T23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="U23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2865,8 +2974,11 @@
       <c r="T24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="U24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2927,8 +3039,11 @@
       <c r="T25" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:20">
+      <c r="U25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2989,8 +3104,11 @@
       <c r="T26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="U26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3051,8 +3169,11 @@
       <c r="T27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="U27" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3113,8 +3234,11 @@
       <c r="T28" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:20">
+      <c r="U28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3175,8 +3299,11 @@
       <c r="T29" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="U29" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3237,8 +3364,11 @@
       <c r="T30" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="U30" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3299,8 +3429,11 @@
       <c r="T31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:20">
+      <c r="U31" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3361,8 +3494,11 @@
       <c r="T32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:20">
+      <c r="U32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3423,8 +3559,11 @@
       <c r="T33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:20">
+      <c r="U33" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3485,8 +3624,11 @@
       <c r="T34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:20">
+      <c r="U34" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3547,8 +3689,11 @@
       <c r="T35" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:20">
+      <c r="U35" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3609,8 +3754,11 @@
       <c r="T36" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:20">
+      <c r="U36" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3671,8 +3819,11 @@
       <c r="T37" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:20">
+      <c r="U37" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3733,8 +3884,11 @@
       <c r="T38" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="1:20">
+      <c r="U38" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3795,8 +3949,11 @@
       <c r="T39" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="1:20">
+      <c r="U39" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3857,8 +4014,11 @@
       <c r="T40" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:20">
+      <c r="U40" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3919,8 +4079,11 @@
       <c r="T41" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="1:20">
+      <c r="U41" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3981,8 +4144,11 @@
       <c r="T42" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="43" spans="1:20">
+      <c r="U42" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4043,8 +4209,11 @@
       <c r="T43" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="44" spans="1:20">
+      <c r="U43" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4105,8 +4274,11 @@
       <c r="T44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:20">
+      <c r="U44" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4167,8 +4339,11 @@
       <c r="T45" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="46" spans="1:20">
+      <c r="U45" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4229,8 +4404,11 @@
       <c r="T46" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="47" spans="1:20">
+      <c r="U46" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4291,8 +4469,11 @@
       <c r="T47" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="48" spans="1:20">
+      <c r="U47" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4353,8 +4534,11 @@
       <c r="T48" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="49" spans="1:20">
+      <c r="U48" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4415,8 +4599,11 @@
       <c r="T49" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="50" spans="1:20">
+      <c r="U49" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
       <c r="A50">
         <v>48</v>
       </c>
@@ -4477,8 +4664,11 @@
       <c r="T50" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="51" spans="1:20">
+      <c r="U50" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4539,8 +4729,11 @@
       <c r="T51" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="52" spans="1:20">
+      <c r="U51" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4601,8 +4794,11 @@
       <c r="T52" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="53" spans="1:20">
+      <c r="U52" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4663,8 +4859,11 @@
       <c r="T53" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="54" spans="1:20">
+      <c r="U53" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4725,8 +4924,11 @@
       <c r="T54" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="55" spans="1:20">
+      <c r="U54" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4787,8 +4989,11 @@
       <c r="T55" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="56" spans="1:20">
+      <c r="U55" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4849,8 +5054,11 @@
       <c r="T56" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="57" spans="1:20">
+      <c r="U56" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4911,8 +5119,11 @@
       <c r="T57" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="58" spans="1:20">
+      <c r="U57" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4973,8 +5184,11 @@
       <c r="T58" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="59" spans="1:20">
+      <c r="U58" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21">
       <c r="A59">
         <v>57</v>
       </c>
@@ -5035,8 +5249,11 @@
       <c r="T59" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="60" spans="1:20">
+      <c r="U59" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21">
       <c r="A60">
         <v>58</v>
       </c>
@@ -5097,8 +5314,11 @@
       <c r="T60" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="61" spans="1:20">
+      <c r="U60" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21">
       <c r="A61">
         <v>59</v>
       </c>
@@ -5159,8 +5379,11 @@
       <c r="T61" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="62" spans="1:20">
+      <c r="U61" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21">
       <c r="A62">
         <v>60</v>
       </c>
@@ -5221,8 +5444,11 @@
       <c r="T62" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="63" spans="1:20">
+      <c r="U62" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21">
       <c r="A63">
         <v>61</v>
       </c>
@@ -5283,8 +5509,11 @@
       <c r="T63" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="64" spans="1:20">
+      <c r="U63" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
       <c r="A64">
         <v>62</v>
       </c>
@@ -5345,8 +5574,11 @@
       <c r="T64" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="65" spans="1:20">
+      <c r="U64" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21">
       <c r="A65">
         <v>63</v>
       </c>
@@ -5407,8 +5639,11 @@
       <c r="T65" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="66" spans="1:20">
+      <c r="U65" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21">
       <c r="A66">
         <v>64</v>
       </c>
@@ -5469,8 +5704,11 @@
       <c r="T66" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="67" spans="1:20">
+      <c r="U66" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21">
       <c r="A67">
         <v>65</v>
       </c>
@@ -5531,8 +5769,11 @@
       <c r="T67" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="68" spans="1:20">
+      <c r="U67" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21">
       <c r="A68">
         <v>66</v>
       </c>
@@ -5593,8 +5834,11 @@
       <c r="T68" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="69" spans="1:20">
+      <c r="U68" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21">
       <c r="A69">
         <v>67</v>
       </c>
@@ -5655,8 +5899,11 @@
       <c r="T69" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="70" spans="1:20">
+      <c r="U69" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21">
       <c r="A70">
         <v>68</v>
       </c>
@@ -5717,8 +5964,11 @@
       <c r="T70" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="71" spans="1:20">
+      <c r="U70" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21">
       <c r="A71">
         <v>69</v>
       </c>
@@ -5779,8 +6029,11 @@
       <c r="T71" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="72" spans="1:20">
+      <c r="U71" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21">
       <c r="A72">
         <v>70</v>
       </c>
@@ -5841,8 +6094,11 @@
       <c r="T72" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="73" spans="1:20">
+      <c r="U72" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21">
       <c r="A73">
         <v>71</v>
       </c>
@@ -5903,8 +6159,11 @@
       <c r="T73" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="74" spans="1:20">
+      <c r="U73" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21">
       <c r="A74">
         <v>72</v>
       </c>
@@ -5965,8 +6224,11 @@
       <c r="T74" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="75" spans="1:20">
+      <c r="U74" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21">
       <c r="A75">
         <v>73</v>
       </c>
@@ -6027,8 +6289,11 @@
       <c r="T75" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="76" spans="1:20">
+      <c r="U75" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21">
       <c r="A76">
         <v>74</v>
       </c>
@@ -6089,8 +6354,11 @@
       <c r="T76" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="77" spans="1:20">
+      <c r="U76" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21">
       <c r="A77">
         <v>75</v>
       </c>
@@ -6151,8 +6419,11 @@
       <c r="T77" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="78" spans="1:20">
+      <c r="U77" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21">
       <c r="A78">
         <v>76</v>
       </c>
@@ -6213,8 +6484,11 @@
       <c r="T78" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="79" spans="1:20">
+      <c r="U78" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21">
       <c r="A79">
         <v>77</v>
       </c>
@@ -6275,8 +6549,11 @@
       <c r="T79" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="80" spans="1:20">
+      <c r="U79" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21">
       <c r="A80">
         <v>78</v>
       </c>
@@ -6337,8 +6614,11 @@
       <c r="T80" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="81" spans="1:20">
+      <c r="U80" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21">
       <c r="A81">
         <v>79</v>
       </c>
@@ -6399,8 +6679,11 @@
       <c r="T81" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="82" spans="1:20">
+      <c r="U81" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21">
       <c r="A82">
         <v>80</v>
       </c>
@@ -6461,8 +6744,11 @@
       <c r="T82" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="83" spans="1:20">
+      <c r="U82" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21">
       <c r="A83">
         <v>81</v>
       </c>
@@ -6523,8 +6809,11 @@
       <c r="T83" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="84" spans="1:20">
+      <c r="U83" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21">
       <c r="A84">
         <v>82</v>
       </c>
@@ -6585,8 +6874,11 @@
       <c r="T84" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="85" spans="1:20">
+      <c r="U84" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21">
       <c r="A85">
         <v>83</v>
       </c>
@@ -6647,8 +6939,11 @@
       <c r="T85" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="86" spans="1:20">
+      <c r="U85" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21">
       <c r="A86">
         <v>84</v>
       </c>
@@ -6709,8 +7004,11 @@
       <c r="T86" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="87" spans="1:20">
+      <c r="U86" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21">
       <c r="A87">
         <v>85</v>
       </c>
@@ -6771,8 +7069,11 @@
       <c r="T87" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="88" spans="1:20">
+      <c r="U87" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21">
       <c r="A88">
         <v>86</v>
       </c>
@@ -6833,8 +7134,11 @@
       <c r="T88" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="89" spans="1:20">
+      <c r="U88" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21">
       <c r="A89">
         <v>87</v>
       </c>
@@ -6895,8 +7199,11 @@
       <c r="T89" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="90" spans="1:20">
+      <c r="U89" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21">
       <c r="A90">
         <v>88</v>
       </c>
@@ -6957,8 +7264,11 @@
       <c r="T90" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="91" spans="1:20">
+      <c r="U90" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21">
       <c r="A91">
         <v>89</v>
       </c>
@@ -7019,8 +7329,11 @@
       <c r="T91" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="92" spans="1:20">
+      <c r="U91" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21">
       <c r="A92">
         <v>90</v>
       </c>
@@ -7081,8 +7394,11 @@
       <c r="T92" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="93" spans="1:20">
+      <c r="U92" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21">
       <c r="A93">
         <v>91</v>
       </c>
@@ -7143,8 +7459,11 @@
       <c r="T93" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="94" spans="1:20">
+      <c r="U93" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21">
       <c r="A94">
         <v>92</v>
       </c>
@@ -7205,8 +7524,11 @@
       <c r="T94" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="95" spans="1:20">
+      <c r="U94" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21">
       <c r="A95">
         <v>93</v>
       </c>
@@ -7265,6 +7587,9 @@
         <v>31</v>
       </c>
       <c r="T95" t="s">
+        <v>31</v>
+      </c>
+      <c r="U95" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change the way of item saved, makes it unique. I think I need more things than I thought to do more
</commit_message>
<xml_diff>
--- a/DataSource/excel/city.xlsx
+++ b/DataSource/excel/city.xlsx
@@ -198,46 +198,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yujie Liu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="2"/>
-            <charset val="134"/>
-          </rPr>
-          <t>贩卖的道具ID，卖掉之后就不再有这个商品了，如果玩家把道具卖入城市，则城市又会出现该道具</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="225">
   <si>
     <t>cityId</t>
   </si>
@@ -912,12 +878,6 @@
   </si>
   <si>
     <t>6;16;53;13</t>
-  </si>
-  <si>
-    <t>sellItemId</t>
-  </si>
-  <si>
-    <t>1;2;3;4;5;6;7;8;9;10;11;12;13;14;15;16</t>
   </si>
 </sst>
 </file>
@@ -1378,13 +1338,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U95"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
+      <selection pane="bottomRight" activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1398,7 +1358,7 @@
     <col min="20" max="20" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1459,11 +1419,8 @@
       <c r="T1" t="s">
         <v>180</v>
       </c>
-      <c r="U1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1524,11 +1481,8 @@
       <c r="T2" t="s">
         <v>10</v>
       </c>
-      <c r="U2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1589,11 +1543,8 @@
       <c r="T3" t="s">
         <v>181</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1654,11 +1605,8 @@
       <c r="T4" t="s">
         <v>31</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1719,11 +1667,8 @@
       <c r="T5" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1784,11 +1729,8 @@
       <c r="T6" t="s">
         <v>31</v>
       </c>
-      <c r="U6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1849,11 +1791,8 @@
       <c r="T7" t="s">
         <v>31</v>
       </c>
-      <c r="U7" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1914,11 +1853,8 @@
       <c r="T8" t="s">
         <v>31</v>
       </c>
-      <c r="U8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1979,11 +1915,8 @@
       <c r="T9" t="s">
         <v>31</v>
       </c>
-      <c r="U9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2044,11 +1977,8 @@
       <c r="T10" t="s">
         <v>31</v>
       </c>
-      <c r="U10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2109,11 +2039,8 @@
       <c r="T11" t="s">
         <v>31</v>
       </c>
-      <c r="U11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2174,11 +2101,8 @@
       <c r="T12" t="s">
         <v>31</v>
       </c>
-      <c r="U12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2239,11 +2163,8 @@
       <c r="T13" t="s">
         <v>31</v>
       </c>
-      <c r="U13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2304,11 +2225,8 @@
       <c r="T14" t="s">
         <v>31</v>
       </c>
-      <c r="U14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2369,11 +2287,8 @@
       <c r="T15" t="s">
         <v>31</v>
       </c>
-      <c r="U15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2434,11 +2349,8 @@
       <c r="T16" t="s">
         <v>31</v>
       </c>
-      <c r="U16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2499,11 +2411,8 @@
       <c r="T17" t="s">
         <v>31</v>
       </c>
-      <c r="U17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2564,11 +2473,8 @@
       <c r="T18" t="s">
         <v>31</v>
       </c>
-      <c r="U18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2629,11 +2535,8 @@
       <c r="T19" t="s">
         <v>31</v>
       </c>
-      <c r="U19" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2694,11 +2597,8 @@
       <c r="T20" t="s">
         <v>31</v>
       </c>
-      <c r="U20" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2759,11 +2659,8 @@
       <c r="T21" t="s">
         <v>31</v>
       </c>
-      <c r="U21" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2824,11 +2721,8 @@
       <c r="T22" t="s">
         <v>31</v>
       </c>
-      <c r="U22" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2889,11 +2783,8 @@
       <c r="T23" t="s">
         <v>31</v>
       </c>
-      <c r="U23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2954,11 +2845,8 @@
       <c r="T24" t="s">
         <v>31</v>
       </c>
-      <c r="U24" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3019,11 +2907,8 @@
       <c r="T25" t="s">
         <v>31</v>
       </c>
-      <c r="U25" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3084,11 +2969,8 @@
       <c r="T26" t="s">
         <v>31</v>
       </c>
-      <c r="U26" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3149,11 +3031,8 @@
       <c r="T27" t="s">
         <v>31</v>
       </c>
-      <c r="U27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3214,11 +3093,8 @@
       <c r="T28" t="s">
         <v>31</v>
       </c>
-      <c r="U28" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3279,11 +3155,8 @@
       <c r="T29" t="s">
         <v>31</v>
       </c>
-      <c r="U29" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3344,11 +3217,8 @@
       <c r="T30" t="s">
         <v>31</v>
       </c>
-      <c r="U30" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3409,11 +3279,8 @@
       <c r="T31" t="s">
         <v>31</v>
       </c>
-      <c r="U31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3474,11 +3341,8 @@
       <c r="T32" t="s">
         <v>31</v>
       </c>
-      <c r="U32" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21">
+    </row>
+    <row r="33" spans="1:20">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3539,11 +3403,8 @@
       <c r="T33" t="s">
         <v>31</v>
       </c>
-      <c r="U33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21">
+    </row>
+    <row r="34" spans="1:20">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3604,11 +3465,8 @@
       <c r="T34" t="s">
         <v>31</v>
       </c>
-      <c r="U34" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
+    </row>
+    <row r="35" spans="1:20">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3669,11 +3527,8 @@
       <c r="T35" t="s">
         <v>31</v>
       </c>
-      <c r="U35" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21">
+    </row>
+    <row r="36" spans="1:20">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3734,11 +3589,8 @@
       <c r="T36" t="s">
         <v>31</v>
       </c>
-      <c r="U36" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21">
+    </row>
+    <row r="37" spans="1:20">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3799,11 +3651,8 @@
       <c r="T37" t="s">
         <v>31</v>
       </c>
-      <c r="U37" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21">
+    </row>
+    <row r="38" spans="1:20">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3864,11 +3713,8 @@
       <c r="T38" t="s">
         <v>31</v>
       </c>
-      <c r="U38" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21">
+    </row>
+    <row r="39" spans="1:20">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3929,11 +3775,8 @@
       <c r="T39" t="s">
         <v>31</v>
       </c>
-      <c r="U39" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21">
+    </row>
+    <row r="40" spans="1:20">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3994,11 +3837,8 @@
       <c r="T40" t="s">
         <v>31</v>
       </c>
-      <c r="U40" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21">
+    </row>
+    <row r="41" spans="1:20">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4059,11 +3899,8 @@
       <c r="T41" t="s">
         <v>31</v>
       </c>
-      <c r="U41" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21">
+    </row>
+    <row r="42" spans="1:20">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4124,11 +3961,8 @@
       <c r="T42" t="s">
         <v>31</v>
       </c>
-      <c r="U42" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21">
+    </row>
+    <row r="43" spans="1:20">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4189,11 +4023,8 @@
       <c r="T43" t="s">
         <v>31</v>
       </c>
-      <c r="U43" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21">
+    </row>
+    <row r="44" spans="1:20">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4254,11 +4085,8 @@
       <c r="T44" t="s">
         <v>31</v>
       </c>
-      <c r="U44" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21">
+    </row>
+    <row r="45" spans="1:20">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4319,11 +4147,8 @@
       <c r="T45" t="s">
         <v>31</v>
       </c>
-      <c r="U45" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21">
+    </row>
+    <row r="46" spans="1:20">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4384,11 +4209,8 @@
       <c r="T46" t="s">
         <v>31</v>
       </c>
-      <c r="U46" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21">
+    </row>
+    <row r="47" spans="1:20">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4449,11 +4271,8 @@
       <c r="T47" t="s">
         <v>31</v>
       </c>
-      <c r="U47" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
+    </row>
+    <row r="48" spans="1:20">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4514,11 +4333,8 @@
       <c r="T48" t="s">
         <v>31</v>
       </c>
-      <c r="U48" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21">
+    </row>
+    <row r="49" spans="1:20">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4579,11 +4395,8 @@
       <c r="T49" t="s">
         <v>31</v>
       </c>
-      <c r="U49" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21">
+    </row>
+    <row r="50" spans="1:20">
       <c r="A50">
         <v>48</v>
       </c>
@@ -4644,11 +4457,8 @@
       <c r="T50" t="s">
         <v>31</v>
       </c>
-      <c r="U50" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21">
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4709,11 +4519,8 @@
       <c r="T51" t="s">
         <v>31</v>
       </c>
-      <c r="U51" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21">
+    </row>
+    <row r="52" spans="1:20">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4774,11 +4581,8 @@
       <c r="T52" t="s">
         <v>31</v>
       </c>
-      <c r="U52" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21">
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4839,11 +4643,8 @@
       <c r="T53" t="s">
         <v>31</v>
       </c>
-      <c r="U53" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21">
+    </row>
+    <row r="54" spans="1:20">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4904,11 +4705,8 @@
       <c r="T54" t="s">
         <v>31</v>
       </c>
-      <c r="U54" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21">
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4969,11 +4767,8 @@
       <c r="T55" t="s">
         <v>31</v>
       </c>
-      <c r="U55" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21">
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56">
         <v>54</v>
       </c>
@@ -5034,11 +4829,8 @@
       <c r="T56" t="s">
         <v>31</v>
       </c>
-      <c r="U56" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21">
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57">
         <v>55</v>
       </c>
@@ -5099,11 +4891,8 @@
       <c r="T57" t="s">
         <v>31</v>
       </c>
-      <c r="U57" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21">
+    </row>
+    <row r="58" spans="1:20">
       <c r="A58">
         <v>56</v>
       </c>
@@ -5164,11 +4953,8 @@
       <c r="T58" t="s">
         <v>31</v>
       </c>
-      <c r="U58" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21">
+    </row>
+    <row r="59" spans="1:20">
       <c r="A59">
         <v>57</v>
       </c>
@@ -5229,11 +5015,8 @@
       <c r="T59" t="s">
         <v>31</v>
       </c>
-      <c r="U59" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21">
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60">
         <v>58</v>
       </c>
@@ -5294,11 +5077,8 @@
       <c r="T60" t="s">
         <v>31</v>
       </c>
-      <c r="U60" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21">
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61">
         <v>59</v>
       </c>
@@ -5359,11 +5139,8 @@
       <c r="T61" t="s">
         <v>31</v>
       </c>
-      <c r="U61" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21">
+    </row>
+    <row r="62" spans="1:20">
       <c r="A62">
         <v>60</v>
       </c>
@@ -5424,11 +5201,8 @@
       <c r="T62" t="s">
         <v>31</v>
       </c>
-      <c r="U62" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21">
+    </row>
+    <row r="63" spans="1:20">
       <c r="A63">
         <v>61</v>
       </c>
@@ -5489,11 +5263,8 @@
       <c r="T63" t="s">
         <v>31</v>
       </c>
-      <c r="U63" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21">
+    </row>
+    <row r="64" spans="1:20">
       <c r="A64">
         <v>62</v>
       </c>
@@ -5554,11 +5325,8 @@
       <c r="T64" t="s">
         <v>31</v>
       </c>
-      <c r="U64" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21">
+    </row>
+    <row r="65" spans="1:20">
       <c r="A65">
         <v>63</v>
       </c>
@@ -5619,11 +5387,8 @@
       <c r="T65" t="s">
         <v>31</v>
       </c>
-      <c r="U65" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21">
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66">
         <v>64</v>
       </c>
@@ -5684,11 +5449,8 @@
       <c r="T66" t="s">
         <v>31</v>
       </c>
-      <c r="U66" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21">
+    </row>
+    <row r="67" spans="1:20">
       <c r="A67">
         <v>65</v>
       </c>
@@ -5749,11 +5511,8 @@
       <c r="T67" t="s">
         <v>31</v>
       </c>
-      <c r="U67" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21">
+    </row>
+    <row r="68" spans="1:20">
       <c r="A68">
         <v>66</v>
       </c>
@@ -5814,11 +5573,8 @@
       <c r="T68" t="s">
         <v>31</v>
       </c>
-      <c r="U68" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21">
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69">
         <v>67</v>
       </c>
@@ -5879,11 +5635,8 @@
       <c r="T69" t="s">
         <v>31</v>
       </c>
-      <c r="U69" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21">
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70">
         <v>68</v>
       </c>
@@ -5944,11 +5697,8 @@
       <c r="T70" t="s">
         <v>31</v>
       </c>
-      <c r="U70" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21">
+    </row>
+    <row r="71" spans="1:20">
       <c r="A71">
         <v>69</v>
       </c>
@@ -6009,11 +5759,8 @@
       <c r="T71" t="s">
         <v>31</v>
       </c>
-      <c r="U71" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21">
+    </row>
+    <row r="72" spans="1:20">
       <c r="A72">
         <v>70</v>
       </c>
@@ -6074,11 +5821,8 @@
       <c r="T72" t="s">
         <v>31</v>
       </c>
-      <c r="U72" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21">
+    </row>
+    <row r="73" spans="1:20">
       <c r="A73">
         <v>71</v>
       </c>
@@ -6139,11 +5883,8 @@
       <c r="T73" t="s">
         <v>31</v>
       </c>
-      <c r="U73" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21">
+    </row>
+    <row r="74" spans="1:20">
       <c r="A74">
         <v>72</v>
       </c>
@@ -6204,11 +5945,8 @@
       <c r="T74" t="s">
         <v>31</v>
       </c>
-      <c r="U74" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21">
+    </row>
+    <row r="75" spans="1:20">
       <c r="A75">
         <v>73</v>
       </c>
@@ -6269,11 +6007,8 @@
       <c r="T75" t="s">
         <v>31</v>
       </c>
-      <c r="U75" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21">
+    </row>
+    <row r="76" spans="1:20">
       <c r="A76">
         <v>74</v>
       </c>
@@ -6334,11 +6069,8 @@
       <c r="T76" t="s">
         <v>31</v>
       </c>
-      <c r="U76" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21">
+    </row>
+    <row r="77" spans="1:20">
       <c r="A77">
         <v>75</v>
       </c>
@@ -6399,11 +6131,8 @@
       <c r="T77" t="s">
         <v>31</v>
       </c>
-      <c r="U77" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21">
+    </row>
+    <row r="78" spans="1:20">
       <c r="A78">
         <v>76</v>
       </c>
@@ -6464,11 +6193,8 @@
       <c r="T78" t="s">
         <v>31</v>
       </c>
-      <c r="U78" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21">
+    </row>
+    <row r="79" spans="1:20">
       <c r="A79">
         <v>77</v>
       </c>
@@ -6529,11 +6255,8 @@
       <c r="T79" t="s">
         <v>31</v>
       </c>
-      <c r="U79" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21">
+    </row>
+    <row r="80" spans="1:20">
       <c r="A80">
         <v>78</v>
       </c>
@@ -6594,11 +6317,8 @@
       <c r="T80" t="s">
         <v>31</v>
       </c>
-      <c r="U80" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:21">
+    </row>
+    <row r="81" spans="1:20">
       <c r="A81">
         <v>79</v>
       </c>
@@ -6659,11 +6379,8 @@
       <c r="T81" t="s">
         <v>31</v>
       </c>
-      <c r="U81" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="82" spans="1:21">
+    </row>
+    <row r="82" spans="1:20">
       <c r="A82">
         <v>80</v>
       </c>
@@ -6724,11 +6441,8 @@
       <c r="T82" t="s">
         <v>31</v>
       </c>
-      <c r="U82" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="83" spans="1:21">
+    </row>
+    <row r="83" spans="1:20">
       <c r="A83">
         <v>81</v>
       </c>
@@ -6789,11 +6503,8 @@
       <c r="T83" t="s">
         <v>31</v>
       </c>
-      <c r="U83" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="1:21">
+    </row>
+    <row r="84" spans="1:20">
       <c r="A84">
         <v>82</v>
       </c>
@@ -6854,11 +6565,8 @@
       <c r="T84" t="s">
         <v>31</v>
       </c>
-      <c r="U84" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="85" spans="1:21">
+    </row>
+    <row r="85" spans="1:20">
       <c r="A85">
         <v>83</v>
       </c>
@@ -6919,11 +6627,8 @@
       <c r="T85" t="s">
         <v>31</v>
       </c>
-      <c r="U85" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="1:21">
+    </row>
+    <row r="86" spans="1:20">
       <c r="A86">
         <v>84</v>
       </c>
@@ -6984,11 +6689,8 @@
       <c r="T86" t="s">
         <v>31</v>
       </c>
-      <c r="U86" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="87" spans="1:21">
+    </row>
+    <row r="87" spans="1:20">
       <c r="A87">
         <v>85</v>
       </c>
@@ -7049,11 +6751,8 @@
       <c r="T87" t="s">
         <v>31</v>
       </c>
-      <c r="U87" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="88" spans="1:21">
+    </row>
+    <row r="88" spans="1:20">
       <c r="A88">
         <v>86</v>
       </c>
@@ -7114,11 +6813,8 @@
       <c r="T88" t="s">
         <v>31</v>
       </c>
-      <c r="U88" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="89" spans="1:21">
+    </row>
+    <row r="89" spans="1:20">
       <c r="A89">
         <v>87</v>
       </c>
@@ -7179,11 +6875,8 @@
       <c r="T89" t="s">
         <v>31</v>
       </c>
-      <c r="U89" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="90" spans="1:21">
+    </row>
+    <row r="90" spans="1:20">
       <c r="A90">
         <v>88</v>
       </c>
@@ -7244,11 +6937,8 @@
       <c r="T90" t="s">
         <v>31</v>
       </c>
-      <c r="U90" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="91" spans="1:21">
+    </row>
+    <row r="91" spans="1:20">
       <c r="A91">
         <v>89</v>
       </c>
@@ -7309,11 +6999,8 @@
       <c r="T91" t="s">
         <v>31</v>
       </c>
-      <c r="U91" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="92" spans="1:21">
+    </row>
+    <row r="92" spans="1:20">
       <c r="A92">
         <v>90</v>
       </c>
@@ -7374,11 +7061,8 @@
       <c r="T92" t="s">
         <v>31</v>
       </c>
-      <c r="U92" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="93" spans="1:21">
+    </row>
+    <row r="93" spans="1:20">
       <c r="A93">
         <v>91</v>
       </c>
@@ -7439,11 +7123,8 @@
       <c r="T93" t="s">
         <v>31</v>
       </c>
-      <c r="U93" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="1:21">
+    </row>
+    <row r="94" spans="1:20">
       <c r="A94">
         <v>92</v>
       </c>
@@ -7504,11 +7185,8 @@
       <c r="T94" t="s">
         <v>31</v>
       </c>
-      <c r="U94" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="95" spans="1:21">
+    </row>
+    <row r="95" spans="1:20">
       <c r="A95">
         <v>93</v>
       </c>
@@ -7567,9 +7245,6 @@
         <v>31</v>
       </c>
       <c r="T95" t="s">
-        <v>31</v>
-      </c>
-      <c r="U95" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add default Dialog format
</commit_message>
<xml_diff>
--- a/DataSource/excel/city.xlsx
+++ b/DataSource/excel/city.xlsx
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="226">
   <si>
     <t>cityId</t>
   </si>
@@ -878,6 +878,9 @@
   </si>
   <si>
     <t>6;16;53;13</t>
+  </si>
+  <si>
+    <t>82_19</t>
   </si>
 </sst>
 </file>
@@ -1341,10 +1344,10 @@
   <dimension ref="A1:T95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T1" sqref="T1:T1048576"/>
+      <selection pane="bottomRight" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1538,7 +1541,7 @@
         <v>185</v>
       </c>
       <c r="S3" t="s">
-        <v>31</v>
+        <v>225</v>
       </c>
       <c r="T3" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
Fix the ship scene conflict bug
solved the music and city background bug
</commit_message>
<xml_diff>
--- a/DataSource/excel/city.xlsx
+++ b/DataSource/excel/city.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26840" windowHeight="20100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="city.csv" sheetId="1" r:id="rId1"/>
@@ -1344,10 +1344,10 @@
   <dimension ref="A1:T95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T7" sqref="T7"/>
+      <selection pane="bottomRight" activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5585,10 +5585,10 @@
         <v>103</v>
       </c>
       <c r="C69" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D69" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E69">
         <v>2</v>

</xml_diff>